<commit_message>
iteration 4 - remise final
</commit_message>
<xml_diff>
--- a/estimation.xlsx
+++ b/estimation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Estimation" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="70">
   <si>
     <t>Définition du noyau (section qui doit obligatoirement être terminée pour réussir le cours : 60%)</t>
   </si>
@@ -204,6 +204,30 @@
   </si>
   <si>
     <t>insertion du nom echoué après plusieurs tentative, insert du nbresurvivant reussit, correctif appliqué à la gestion des widths (max et min)</t>
+  </si>
+  <si>
+    <t>ajout taux protection, détails dans ressources. Création de l'activity "Survivant", tentative de création d'un survivant et lajouter dans une liste ensuite et afficher cette liste dans une listView</t>
+  </si>
+  <si>
+    <t>beaucoup de correction appliqués dans cette itération, ajout dune base de donnée</t>
+  </si>
+  <si>
+    <t>4.5</t>
+  </si>
+  <si>
+    <t>gestion de lactivité survivant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gestion de la suppression dun survivant </t>
+  </si>
+  <si>
+    <t>7.5</t>
+  </si>
+  <si>
+    <t>tentative correction supprimerUser dans activité</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ajout de lactivity survivant qui permet dafficher les données des survivants. Gestion des relative/linear layout mieux executer car plus de compréhension qu'au début du projet. </t>
   </si>
 </sst>
 </file>
@@ -2163,7 +2187,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:C47"/>
   <sheetViews>
-    <sheetView showWhiteSpace="0" view="pageLayout" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showWhiteSpace="0" view="pageLayout" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B42" sqref="B42:B47"/>
     </sheetView>
   </sheetViews>
@@ -2448,8 +2472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:C47"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView view="pageLayout" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42:B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2583,7 +2607,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" s="4"/>
+      <c r="A21" s="18"/>
       <c r="B21" s="4"/>
       <c r="C21" s="15"/>
     </row>
@@ -2682,7 +2706,9 @@
       <c r="A40" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B40" s="4"/>
+      <c r="B40" s="4">
+        <v>6</v>
+      </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="7"/>
@@ -2691,7 +2717,9 @@
       <c r="A42" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B42" s="21"/>
+      <c r="B42" s="21" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B43" s="22"/>
@@ -2723,8 +2751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:C47"/>
   <sheetViews>
-    <sheetView showWhiteSpace="0" view="pageLayout" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" topLeftCell="A39" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42:B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2781,24 +2809,48 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" s="12"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="15"/>
+      <c r="A14" s="12">
+        <v>43226</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="15"/>
+      <c r="A15" s="18">
+        <v>43227</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="15"/>
+      <c r="A16" s="18">
+        <v>43228</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" s="15">
+        <v>3</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="15"/>
+      <c r="A17" s="18">
+        <v>43234</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="4"/>
@@ -2902,7 +2954,7 @@
       <c r="B37" s="20"/>
       <c r="C37" s="16">
         <f>SUM(C14:C36)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -2915,7 +2967,9 @@
       <c r="A40" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B40" s="4"/>
+      <c r="B40" s="4">
+        <v>8</v>
+      </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="7"/>
@@ -2924,7 +2978,9 @@
       <c r="A42" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B42" s="21"/>
+      <c r="B42" s="21" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B43" s="22"/>

</xml_diff>